<commit_message>
Replace with row insert and update date format
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>CONSULTANT WEEKLY TIMESHEET</t>
   </si>
@@ -31,7 +31,7 @@
     <t>End Date</t>
   </si>
   <si>
-    <t>04-12-2023</t>
+    <t>04/12/2023</t>
   </si>
   <si>
     <t>Date</t>
@@ -58,7 +58,7 @@
     <t>Total Time</t>
   </si>
   <si>
-    <t>Total Hours per day</t>
+    <t>Total Hours per Day</t>
   </si>
   <si>
     <t>meeting</t>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>api defenition</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>discussion</t>
@@ -475,9 +472,6 @@
       <c r="F8" t="s">
         <v>17</v>
       </c>
-      <c r="G8" t="s">
-        <v>18</v>
-      </c>
       <c r="H8">
         <v>1</v>
       </c>
@@ -496,16 +490,13 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
         <v>19</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>20</v>
-      </c>
-      <c r="F9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" t="s">
-        <v>18</v>
       </c>
       <c r="H9">
         <v>2</v>
@@ -525,16 +516,13 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
         <v>22</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>23</v>
-      </c>
-      <c r="F10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" t="s">
-        <v>18</v>
       </c>
       <c r="H10">
         <v>4</v>
@@ -548,12 +536,16 @@
     </row>
     <row r="13">
       <c r="I13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J13">
         <v>7</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
 </worksheet>
 </file>
</xml_diff>